<commit_message>
Updated planning with new hours
</commit_message>
<xml_diff>
--- a/documentation/planning/Urenplanning en verantwoording themaopdracht Devices.xlsx
+++ b/documentation/planning/Urenplanning en verantwoording themaopdracht Devices.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\ClionProjects\B1-BAZEN-THEMA-DEVICES\documentation\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\Dropbox\b1 programming\TI jaar 2\thema devices project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="50">
   <si>
     <t>lesweek</t>
   </si>
@@ -98,67 +98,79 @@
     <t>Bart van der Kolk</t>
   </si>
   <si>
-    <t>Klassen diagram bespreken</t>
-  </si>
-  <si>
-    <t>Klassen diagram opzetten</t>
-  </si>
-  <si>
-    <t>concurency model opzetten</t>
-  </si>
-  <si>
-    <t>STD tekenen</t>
-  </si>
-  <si>
-    <t>Planning doornemen en alles klaar zetten</t>
-  </si>
-  <si>
-    <t>C++ omgeving klaar maken</t>
-  </si>
-  <si>
-    <t>hardware opzetten</t>
-  </si>
-  <si>
-    <t>resultaten bespreken en aanpassen</t>
-  </si>
-  <si>
-    <t>Receiver class progammeren</t>
-  </si>
-  <si>
-    <t>Transmitter class progammeren</t>
-  </si>
-  <si>
-    <t>Uitzoeken hoe we de receiver en transmitter gaan laten samen werken</t>
-  </si>
-  <si>
-    <t>keypad class opzetten</t>
-  </si>
-  <si>
-    <t>oled display class opzetten</t>
-  </si>
-  <si>
-    <t>score class opzetten</t>
-  </si>
-  <si>
-    <t>spel leider class opzetten</t>
-  </si>
-  <si>
-    <t>gametimer class opzetten</t>
-  </si>
-  <si>
-    <t>speler class opzetten</t>
-  </si>
-  <si>
-    <t>spel leider class uitwerken</t>
-  </si>
-  <si>
-    <t>Speler en spelleider class uit testen en debuggen + documenteren</t>
-  </si>
-  <si>
-    <t>Onderzoek implementatie concurrency mechanismen door open source RTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Gezamenlijk casus door lezen</t>
+  </si>
+  <si>
+    <t>CRC sessie</t>
+  </si>
+  <si>
+    <t>klassendiagram</t>
+  </si>
+  <si>
+    <t>uitwerkingen ui schermen</t>
+  </si>
+  <si>
+    <t>c++ omgeving opgezet</t>
+  </si>
+  <si>
+    <t>taaktabel</t>
+  </si>
+  <si>
+    <t>concurrencydiagram</t>
+  </si>
+  <si>
+    <t>statetransitiondiagram</t>
+  </si>
+  <si>
+    <t>onderzoeksrapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transmitter/receiver nul versie uitbreiding </t>
+  </si>
+  <si>
+    <t>voortgangsgesprek</t>
+  </si>
+  <si>
+    <t>laatste feedback aanpassen op de SA</t>
+  </si>
+  <si>
+    <t>eerste c++ code schrijven gebaseerd op de SA</t>
+  </si>
+  <si>
+    <t>taken verdeling voor uitwerken klassen diagram naar c++ code</t>
+  </si>
+  <si>
+    <t>werken aan de c++ code klassen</t>
+  </si>
+  <si>
+    <t>werken aan onderzoeksrapport</t>
+  </si>
+  <si>
+    <t>voortganggesprek</t>
+  </si>
+  <si>
+    <t>eventuele aanpassingen aan onderzoeksrapport</t>
+  </si>
+  <si>
+    <t>samenvoeging van alle c++ classen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testen/verbeteren van de c++ code </t>
+  </si>
+  <si>
+    <t>code vergelijken met de SA en hier gelijkheid inmaken</t>
+  </si>
+  <si>
+    <t>hardware opbouwen</t>
+  </si>
+  <si>
+    <t>tentamen</t>
+  </si>
+  <si>
+    <t>StateManagment systeem en receiver listener progammeren</t>
+  </si>
+  <si>
+    <t>fouten inzien solution architecture</t>
   </si>
 </sst>
 </file>
@@ -488,6 +500,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -497,7 +510,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L130"/>
+  <dimension ref="A1:L128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -885,22 +897,22 @@
       <c r="A3" s="27"/>
       <c r="B3" s="32"/>
       <c r="C3" s="33"/>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="44"/>
+      <c r="F3" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="44"/>
+      <c r="K3" s="45"/>
       <c r="L3" s="35" t="s">
         <v>19</v>
       </c>
@@ -959,30 +971,14 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
@@ -990,32 +986,28 @@
         <v>42667</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2</v>
       </c>
       <c r="F7" s="18">
-        <v>1</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>7</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G7" s="18"/>
       <c r="H7" s="22">
-        <v>1</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="I7" s="22">
+        <v>2</v>
       </c>
       <c r="J7" s="19">
-        <v>1</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
@@ -1023,32 +1015,28 @@
         <v>42667</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>7</v>
+      <c r="E8" s="9">
+        <v>1</v>
       </c>
       <c r="F8" s="18">
         <v>1</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>7</v>
-      </c>
+      <c r="G8" s="18"/>
       <c r="H8" s="22">
         <v>1</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>7</v>
+      <c r="I8" s="22">
+        <v>1</v>
       </c>
       <c r="J8" s="19">
         <v>1</v>
       </c>
-      <c r="K8" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
@@ -1056,31 +1044,31 @@
         <v>42667</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="9">
         <v>4</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>7</v>
+      <c r="E9" s="9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="18">
+        <v>4</v>
+      </c>
+      <c r="G9" s="18">
+        <v>5</v>
+      </c>
+      <c r="H9" s="22">
+        <v>4</v>
+      </c>
+      <c r="I9" s="22">
+        <v>4</v>
+      </c>
+      <c r="J9" s="19">
+        <v>4</v>
+      </c>
+      <c r="K9" s="19">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1089,32 +1077,28 @@
         <v>42667</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="18">
+        <v>1</v>
+      </c>
+      <c r="G10" s="18">
+        <v>1</v>
       </c>
       <c r="H10" s="22">
-        <v>4</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I10" s="22">
+        <v>1</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
@@ -1122,131 +1106,99 @@
         <v>42667</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="19">
-        <v>4</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="3">
-        <v>42667</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="18">
+        <v>42668</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>7</v>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="22">
+        <v>2</v>
+      </c>
+      <c r="I12" s="22">
+        <v>3</v>
+      </c>
+      <c r="J12" s="19">
+        <v>2</v>
+      </c>
+      <c r="K12" s="19">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="3">
-        <v>42667</v>
+        <v>42668</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="18">
-        <v>2</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="22">
+        <v>1</v>
+      </c>
+      <c r="I13" s="22">
+        <v>1</v>
+      </c>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="3">
-        <v>42667</v>
+        <v>42668</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="9">
-        <v>2</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="18">
-        <v>2</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="22">
-        <v>2</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="19">
-        <v>2</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I14" s="22">
+        <v>3</v>
+      </c>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
@@ -1254,27 +1206,19 @@
         <v>42668</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="9">
-        <v>4</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="18">
-        <v>4</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>7</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="22"/>
-      <c r="I15" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19" t="s">
-        <v>7</v>
+      <c r="I15" s="22"/>
+      <c r="J15" s="19">
+        <v>3</v>
+      </c>
+      <c r="K15" s="19">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1283,32 +1227,22 @@
         <v>42668</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="22">
-        <v>4</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="19">
-        <v>4</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9">
+        <v>3</v>
+      </c>
+      <c r="F16" s="18">
+        <v>8</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22">
+        <v>3</v>
+      </c>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
@@ -1316,441 +1250,355 @@
         <v>42668</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="9">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="18">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E17" s="9">
+        <v>4</v>
+      </c>
+      <c r="F17" s="18"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="22">
-        <v>1</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="19">
-        <v>1</v>
-      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="19"/>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="3">
-        <v>42668</v>
+        <v>42669</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="9">
-        <v>3</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="22">
+        <v>1</v>
+      </c>
+      <c r="I18" s="22">
+        <v>1</v>
+      </c>
+      <c r="J18" s="19">
+        <v>1</v>
+      </c>
+      <c r="K18" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="3">
-        <v>42668</v>
+        <v>42669</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>7</v>
+        <v>49</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>3</v>
       </c>
       <c r="F19" s="18">
+        <v>2</v>
+      </c>
+      <c r="G19" s="18">
+        <v>2</v>
+      </c>
+      <c r="H19" s="22">
+        <v>2</v>
+      </c>
+      <c r="I19" s="22">
         <v>3</v>
       </c>
-      <c r="G19" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="22">
+      <c r="J19" s="19">
+        <v>2</v>
+      </c>
+      <c r="K19" s="19">
         <v>3</v>
       </c>
-      <c r="I19" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3">
-        <v>42668</v>
+        <v>42669</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="18">
+        <v>8</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="3">
-        <v>42668</v>
+        <v>42670</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="19">
+        <v>33</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9">
         <v>3</v>
       </c>
-      <c r="K21" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22">
+        <v>4</v>
+      </c>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="3">
-        <v>42669</v>
+        <v>42670</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="19">
-        <v>2</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9">
+        <v>4</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="3">
-        <v>42669</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="18">
-        <v>8</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>7</v>
-      </c>
+        <v>42671</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="9">
+        <v>5</v>
+      </c>
+      <c r="E23" s="9">
+        <v>5</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="22">
-        <v>8</v>
-      </c>
-      <c r="I23" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="I23" s="22">
+        <v>5</v>
+      </c>
+      <c r="J23" s="19">
+        <v>5</v>
+      </c>
+      <c r="K23" s="19">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="3">
-        <v>42669</v>
+        <v>42671</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D24" s="9">
-        <v>8</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="19">
+        <v>5</v>
+      </c>
+      <c r="E24" s="9">
         <v>6</v>
       </c>
-      <c r="K24" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="3">
-        <v>42670</v>
+        <v>42673</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="9">
-        <v>8</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="18">
-        <v>8</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="22">
-        <v>8</v>
-      </c>
-      <c r="I25" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" s="19">
-        <v>8</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>7</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9">
+        <v>3</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="3">
-        <v>42671</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="9">
-        <v>8</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="18">
-        <v>8</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="22">
-        <v>8</v>
-      </c>
-      <c r="I26" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J26" s="19">
-        <v>8</v>
-      </c>
-      <c r="K26" s="19" t="s">
-        <v>45</v>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="7">
+        <f>SUM(D6:D24)</f>
+        <v>29</v>
+      </c>
+      <c r="E26" s="7">
+        <f>SUM(E6:E25)</f>
+        <v>47</v>
+      </c>
+      <c r="F26" s="7">
+        <f>SUM(F6:F24)</f>
+        <v>27</v>
+      </c>
+      <c r="G26" s="7">
+        <f>SUM(G6:G19)</f>
+        <v>9</v>
+      </c>
+      <c r="H26" s="7">
+        <f>SUM(H6:H24)</f>
+        <v>22</v>
+      </c>
+      <c r="I26" s="7">
+        <f>SUM(I6:I24)</f>
+        <v>31</v>
+      </c>
+      <c r="J26" s="7">
+        <f>SUM(J6:J24)</f>
+        <v>20</v>
+      </c>
+      <c r="K26" s="7">
+        <f>SUM(K6:K24)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="A27" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3">
+        <v>42674</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="22">
+        <v>1</v>
+      </c>
+      <c r="I27" s="22"/>
+      <c r="J27" s="19">
+        <v>1</v>
+      </c>
+      <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="7">
-        <f>SUM(D6:D27)</f>
+      <c r="A28" s="10"/>
+      <c r="B28" s="3">
+        <v>42674</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="9">
+        <v>6</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="22">
+        <v>6</v>
+      </c>
+      <c r="I28" s="22"/>
+      <c r="J28" s="19">
+        <v>6</v>
+      </c>
+      <c r="K28" s="19"/>
+    </row>
+    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="3">
+        <v>42674</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="7">
-        <f>SUM(E6:E23)</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
-        <f>SUM(F6:F27)</f>
-        <v>40</v>
-      </c>
-      <c r="G28" s="7">
-        <f>SUM(G6:G23)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="7">
-        <f>SUM(H6:H27)</f>
-        <v>40</v>
-      </c>
-      <c r="I28" s="7">
-        <f>SUM(I6:I23)</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="7">
-        <f>SUM(J6:J27)</f>
-        <v>40</v>
-      </c>
-      <c r="K28" s="7">
-        <f>SUM(K6:K23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="D29" s="9"/>
       <c r="E29" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="22" t="s">
-        <v>7</v>
-      </c>
+      <c r="F29" s="18">
+        <v>7</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J29" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="J29" s="19"/>
       <c r="K29" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="9" t="s">
-        <v>7</v>
+      <c r="B30" s="3">
+        <v>42674</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="9">
+        <v>1</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="18" t="s">
-        <v>7</v>
+      <c r="F30" s="18">
+        <v>1</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="22" t="s">
-        <v>7</v>
+      <c r="H30" s="22">
+        <v>1</v>
       </c>
       <c r="I30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J30" s="19" t="s">
-        <v>7</v>
+      <c r="J30" s="19">
+        <v>1</v>
       </c>
       <c r="K30" s="19" t="s">
         <v>7</v>
@@ -1758,28 +1606,32 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="9" t="s">
-        <v>7</v>
+      <c r="B31" s="3">
+        <v>42675</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="9">
+        <v>2</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="18" t="s">
-        <v>7</v>
+      <c r="F31" s="18">
+        <v>2</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="22" t="s">
-        <v>7</v>
+      <c r="H31" s="22">
+        <v>2</v>
       </c>
       <c r="I31" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J31" s="19" t="s">
-        <v>7</v>
+      <c r="J31" s="19">
+        <v>2</v>
       </c>
       <c r="K31" s="19" t="s">
         <v>7</v>
@@ -1787,28 +1639,32 @@
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="9" t="s">
-        <v>7</v>
+      <c r="B32" s="3">
+        <v>42675</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="9">
+        <v>2</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="18" t="s">
-        <v>7</v>
+      <c r="F32" s="18">
+        <v>2</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="22" t="s">
-        <v>7</v>
+      <c r="H32" s="22">
+        <v>2</v>
       </c>
       <c r="I32" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J32" s="19" t="s">
-        <v>7</v>
+      <c r="J32" s="19">
+        <v>2</v>
       </c>
       <c r="K32" s="19" t="s">
         <v>7</v>
@@ -1816,28 +1672,32 @@
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="9" t="s">
-        <v>7</v>
+      <c r="B33" s="3">
+        <v>42675</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="9">
+        <v>1</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="18" t="s">
-        <v>7</v>
+      <c r="F33" s="18">
+        <v>1</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="22" t="s">
-        <v>7</v>
+      <c r="H33" s="22">
+        <v>1</v>
       </c>
       <c r="I33" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J33" s="19" t="s">
-        <v>7</v>
+      <c r="J33" s="19">
+        <v>1</v>
       </c>
       <c r="K33" s="19" t="s">
         <v>7</v>
@@ -1845,28 +1705,32 @@
     </row>
     <row r="34" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="9" t="s">
-        <v>7</v>
+      <c r="B34" s="3">
+        <v>42676</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="9">
+        <v>4</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="18" t="s">
-        <v>7</v>
+      <c r="F34" s="18">
+        <v>4</v>
       </c>
       <c r="G34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="22" t="s">
-        <v>7</v>
+      <c r="H34" s="22">
+        <v>4</v>
       </c>
       <c r="I34" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="19" t="s">
-        <v>7</v>
+      <c r="J34" s="19">
+        <v>4</v>
       </c>
       <c r="K34" s="19" t="s">
         <v>7</v>
@@ -1874,28 +1738,32 @@
     </row>
     <row r="35" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="9" t="s">
-        <v>7</v>
+      <c r="B35" s="3">
+        <v>42676</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="9">
+        <v>4</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="18" t="s">
-        <v>7</v>
+      <c r="F35" s="18">
+        <v>4</v>
       </c>
       <c r="G35" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="22" t="s">
-        <v>7</v>
+      <c r="H35" s="22">
+        <v>4</v>
       </c>
       <c r="I35" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J35" s="19" t="s">
-        <v>7</v>
+      <c r="J35" s="19">
+        <v>4</v>
       </c>
       <c r="K35" s="19" t="s">
         <v>7</v>
@@ -1903,8 +1771,12 @@
     </row>
     <row r="36" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="3">
+        <v>42677</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="D36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1932,8 +1804,12 @@
     </row>
     <row r="37" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="3">
+        <v>42678</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="D37" s="9" t="s">
         <v>7</v>
       </c>
@@ -2047,37 +1923,49 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>7</v>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" ref="D41:K41" si="0">SUM(D27:D39)</f>
+        <v>21</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G41" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="3"/>
       <c r="C42" s="4"/>
       <c r="D42" s="9" t="s">
         <v>7</v>
@@ -2105,48 +1993,36 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="7">
-        <f t="shared" ref="D43:K43" si="0">SUM(D29:D41)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A43" s="11"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="A44" s="11"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
       <c r="D44" s="9" t="s">
@@ -2175,7 +2051,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
       <c r="D45" s="9" t="s">
@@ -2204,7 +2080,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
       <c r="D46" s="9" t="s">
@@ -2349,153 +2225,121 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="10"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J51" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K51" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J52" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K52" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="6" t="s">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="7">
-        <f t="shared" ref="D53:K53" si="1">SUM(D44:D52)</f>
+      <c r="D51" s="7">
+        <f t="shared" ref="D51:K51" si="1">SUM(D42:D50)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E51" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F51" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G53" s="7">
+      <c r="G51" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H51" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I53" s="7">
+      <c r="I51" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J53" s="7">
+      <c r="J51" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K53" s="7">
+      <c r="K51" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
+    <row r="52" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+    </row>
+    <row r="53" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="21">
+        <f>SUM(D51,D26,D41)</f>
+        <v>50</v>
+      </c>
+      <c r="E53" s="21">
+        <f t="shared" ref="E53:K53" si="2">SUM(E51,E26,E41)</f>
+        <v>47</v>
+      </c>
+      <c r="F53" s="20">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="G53" s="20">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="H53" s="23">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="I53" s="23">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="J53" s="24">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="K53" s="24">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
     <row r="54" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
     </row>
     <row r="55" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="21">
-        <f>SUM(D53,D28,D43)</f>
-        <v>40</v>
-      </c>
-      <c r="E55" s="21">
-        <f t="shared" ref="E55:K55" si="2">SUM(E53,E28,E43)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="20">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="G55" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H55" s="23">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="I55" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J55" s="24">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="K55" s="24">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
@@ -3445,32 +3289,6 @@
       <c r="I128" s="17"/>
       <c r="J128" s="17"/>
       <c r="K128" s="17"/>
-    </row>
-    <row r="129" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="17"/>
-      <c r="B129" s="17"/>
-      <c r="C129" s="17"/>
-      <c r="D129" s="17"/>
-      <c r="E129" s="17"/>
-      <c r="F129" s="17"/>
-      <c r="G129" s="17"/>
-      <c r="H129" s="17"/>
-      <c r="I129" s="17"/>
-      <c r="J129" s="17"/>
-      <c r="K129" s="17"/>
-    </row>
-    <row r="130" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="17"/>
-      <c r="B130" s="17"/>
-      <c r="C130" s="17"/>
-      <c r="D130" s="17"/>
-      <c r="E130" s="17"/>
-      <c r="F130" s="17"/>
-      <c r="G130" s="17"/>
-      <c r="H130" s="17"/>
-      <c r="I130" s="17"/>
-      <c r="J130" s="17"/>
-      <c r="K130" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3729,9 +3547,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29FDA2D9-0F29-4761-875B-F7795DA98BB3}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>